<commit_message>
Crating excel file in the project for counting test run number
</commit_message>
<xml_diff>
--- a/TestRunCounter.xlsx
+++ b/TestRunCounter.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\IdeaProjects\POMStructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE581C57-924D-4DC2-9BB4-C15B8D6469F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEFF23D-1E22-4153-8D93-095CF27756FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,15 +17,11 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -359,14 +355,14 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="n">
-        <v>32.0</v>
+      <c r="A1" s="3">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -376,7 +372,7 @@
       <c r="H8" s="1"/>
     </row>
     <row r="36" spans="21:21" x14ac:dyDescent="0.25">
-      <c r="U36" s="0">
+      <c r="U36">
         <v>4</v>
       </c>
     </row>

</xml_diff>